<commit_message>
made instructions for the actual experiment, with separated pages. Made script for loading the instruction for all phases (key_prac unfinished). Made function for study phase, to be tested.
</commit_message>
<xml_diff>
--- a/stmuli/genetic_180_rand_jitter_run9045.xlsx
+++ b/stmuli/genetic_180_rand_jitter_run9045.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AFE1723-660D-4BAA-8C69-79BE7AC08816}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222E3030-FCDF-4708-BEE8-40A31E71E914}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9444" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1study_jitter" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5112" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5124" uniqueCount="192">
   <si>
     <t>concepts</t>
   </si>
@@ -596,6 +596,15 @@
   </si>
   <si>
     <t>norm_fam</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -5276,10 +5285,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X451"/>
+  <dimension ref="A1:X456"/>
   <sheetViews>
-    <sheetView topLeftCell="D240" workbookViewId="0">
-      <selection activeCell="M255" sqref="M255"/>
+    <sheetView topLeftCell="F443" workbookViewId="0">
+      <selection activeCell="T454" sqref="T454:T456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -33260,6 +33269,69 @@
       </c>
       <c r="W451">
         <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="454" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" t="s">
+        <v>189</v>
+      </c>
+      <c r="B454">
+        <f>AVERAGE(B2:B451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="H454">
+        <f>AVERAGE(H2:H451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="N454">
+        <f>AVERAGE(N2:N451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="T454">
+        <f>AVERAGE(T2:T451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+    </row>
+    <row r="455" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" t="s">
+        <v>190</v>
+      </c>
+      <c r="B455">
+        <f>MIN(B2:B451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="H455">
+        <f>MIN(H2:H451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="N455">
+        <f>MIN(N2:N451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="T455">
+        <f>MIN(T2:T451)</f>
+        <v>1.00049871904147</v>
+      </c>
+    </row>
+    <row r="456" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" t="s">
+        <v>191</v>
+      </c>
+      <c r="B456">
+        <f>MAX(B2:B451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="H456">
+        <f>MAX(H2:H451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="N456">
+        <f>MAX(N2:N451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="T456">
+        <f>MAX(T2:T451)</f>
+        <v>3.9599118628268202</v>
       </c>
     </row>
   </sheetData>
@@ -33672,10 +33744,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57707210-E57B-49AC-9F45-3A7C6A28F2F3}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="G184" sqref="G184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -40559,6 +40631,45 @@
       </c>
       <c r="L181">
         <v>6.85</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" t="s">
+        <v>189</v>
+      </c>
+      <c r="B184">
+        <f>AVERAGE(B2:B181)</f>
+        <v>4.0321259810805419</v>
+      </c>
+      <c r="H184">
+        <f>AVERAGE(H2:H181)</f>
+        <v>4.0321259810805419</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" t="s">
+        <v>190</v>
+      </c>
+      <c r="B185">
+        <f>MIN(B2:B181)</f>
+        <v>2.5093045562573599</v>
+      </c>
+      <c r="H185">
+        <f>MIN(H2:H181)</f>
+        <v>2.5093045562573599</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" t="s">
+        <v>191</v>
+      </c>
+      <c r="B186">
+        <f>MAX(B2:B181)</f>
+        <v>9.2200592316688894</v>
+      </c>
+      <c r="H186">
+        <f>MAX(H2:H181)</f>
+        <v>9.2200592316688894</v>
       </c>
     </row>
   </sheetData>
@@ -40842,10 +40953,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B151772-C1CA-4FA6-8165-0F952CDA973F}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:X451"/>
+  <dimension ref="A1:X456"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I457" sqref="I457"/>
+    <sheetView topLeftCell="A444" workbookViewId="0">
+      <selection activeCell="A456" sqref="A456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -68822,6 +68933,69 @@
       </c>
       <c r="W451">
         <v>5.7</v>
+      </c>
+    </row>
+    <row r="454" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" t="s">
+        <v>189</v>
+      </c>
+      <c r="B454">
+        <f>AVERAGE(B2:B451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="H454">
+        <f>AVERAGE(H2:H451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="N454">
+        <f>AVERAGE(N2:N451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+      <c r="T454">
+        <f>AVERAGE(T2:T451)</f>
+        <v>1.5063448747403199</v>
+      </c>
+    </row>
+    <row r="455" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" t="s">
+        <v>190</v>
+      </c>
+      <c r="B455">
+        <f>MIN(B2:B451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="H455">
+        <f>MIN(H2:H451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="N455">
+        <f>MIN(N2:N451)</f>
+        <v>1.00049871904147</v>
+      </c>
+      <c r="T455">
+        <f>MIN(T2:T451)</f>
+        <v>1.00049871904147</v>
+      </c>
+    </row>
+    <row r="456" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" t="s">
+        <v>191</v>
+      </c>
+      <c r="B456">
+        <f>MAX(B2:B451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="H456">
+        <f>MAX(H2:H451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="N456">
+        <f>MAX(N2:N451)</f>
+        <v>3.9599118628268202</v>
+      </c>
+      <c r="T456">
+        <f>MAX(T2:T451)</f>
+        <v>3.9599118628268202</v>
       </c>
     </row>
   </sheetData>
@@ -68873,7 +69047,7 @@
   <conditionalFormatting sqref="A434 A416:A432">
     <cfRule type="duplicateValues" dxfId="199" priority="116"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A435:A451 A433">
+  <conditionalFormatting sqref="A435:A451 A433 A454:A456">
     <cfRule type="duplicateValues" dxfId="198" priority="117"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A362:A379">
@@ -69215,10 +69389,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673A43C1-0202-4750-9CCA-49EE1BC11C37}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L181"/>
+  <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="H184" sqref="H184:H186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -76104,6 +76278,45 @@
       </c>
       <c r="L181" s="1">
         <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B184">
+        <f>AVERAGE(B2:B181)</f>
+        <v>4.0321259810805419</v>
+      </c>
+      <c r="H184">
+        <f>AVERAGE(H2:H181)</f>
+        <v>4.0321259810805419</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B185">
+        <f>MIN(B2:B181)</f>
+        <v>2.5093045562573599</v>
+      </c>
+      <c r="H185">
+        <f>MIN(H2:H181)</f>
+        <v>2.5093045562573599</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B186">
+        <f>MAX(B2:B181)</f>
+        <v>9.2200592316688894</v>
+      </c>
+      <c r="H186">
+        <f>MAX(H2:H181)</f>
+        <v>9.2200592316688894</v>
       </c>
     </row>
   </sheetData>
@@ -76239,7 +76452,7 @@
   <conditionalFormatting sqref="A172:A176">
     <cfRule type="duplicateValues" dxfId="46" priority="47"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A177:A181">
+  <conditionalFormatting sqref="A177:A181 A184:A186">
     <cfRule type="duplicateValues" dxfId="45" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G6">

</xml_diff>

<commit_message>
fixed 005 020 022 with normative ratings, added 1 vs. 789 in study phase
</commit_message>
<xml_diff>
--- a/stmuli/genetic_180_rand_jitter_run9045.xlsx
+++ b/stmuli/genetic_180_rand_jitter_run9045.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222E3030-FCDF-4708-BEE8-40A31E71E914}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBEE6D8-466B-4CFF-AFBB-484565AB7148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="9444" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1644" yWindow="1422" windowWidth="18612" windowHeight="9030" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1study_jitter" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -69391,8 +69394,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="H184" sqref="H184:H186"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="K186" sqref="K186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -76288,10 +76291,18 @@
         <f>AVERAGE(B2:B181)</f>
         <v>4.0321259810805419</v>
       </c>
+      <c r="F184">
+        <f>AVERAGE(F2:F181)</f>
+        <v>5.8733333333333348</v>
+      </c>
       <c r="H184">
         <f>AVERAGE(H2:H181)</f>
         <v>4.0321259810805419</v>
       </c>
+      <c r="L184">
+        <f>AVERAGE(F2:F181)</f>
+        <v>5.8733333333333348</v>
+      </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
@@ -76301,10 +76312,18 @@
         <f>MIN(B2:B181)</f>
         <v>2.5093045562573599</v>
       </c>
+      <c r="F185">
+        <f>MIN(F2:F18)</f>
+        <v>1.75</v>
+      </c>
       <c r="H185">
         <f>MIN(H2:H181)</f>
         <v>2.5093045562573599</v>
       </c>
+      <c r="L185">
+        <f>MIN(L2:L181)</f>
+        <v>1.75</v>
+      </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
@@ -76314,9 +76333,17 @@
         <f>MAX(B2:B181)</f>
         <v>9.2200592316688894</v>
       </c>
+      <c r="F186">
+        <f>MAX(F2:F181)</f>
+        <v>8.9499999999999993</v>
+      </c>
       <c r="H186">
         <f>MAX(H2:H181)</f>
         <v>9.2200592316688894</v>
+      </c>
+      <c r="L186">
+        <f>MAX(L2:L181)</f>
+        <v>8.9499999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testphase all3 linear contrast script, enforcing contrast vector to sum to 0 within each run
</commit_message>
<xml_diff>
--- a/stmuli/genetic_180_rand_jitter_run9045.xlsx
+++ b/stmuli/genetic_180_rand_jitter_run9045.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBEE6D8-466B-4CFF-AFBB-484565AB7148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C1116B-7B09-4BF9-B7AC-E982B96C22E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1644" yWindow="1422" windowWidth="18612" windowHeight="9030" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5124" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5128" uniqueCount="196">
   <si>
     <t>concepts</t>
   </si>
@@ -609,6 +609,18 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>1/5</t>
+  </si>
+  <si>
+    <t>2/5</t>
+  </si>
+  <si>
+    <t>3/5</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
 </sst>
 </file>
 
@@ -656,9 +668,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -69392,10 +69405,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{673A43C1-0202-4750-9CCA-49EE1BC11C37}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:L186"/>
+  <dimension ref="A1:L190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="K186" sqref="K186"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="E192" sqref="E192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -76344,6 +76357,42 @@
       <c r="L186">
         <f>MAX(L2:L181)</f>
         <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F187">
+        <f>(F186-F185)/5+F185</f>
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F188">
+        <f>2*(F186-F185)/5+F185</f>
+        <v>4.63</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F189">
+        <f>3*(F186-F185)/5+F185</f>
+        <v>6.0699999999999994</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F190">
+        <f>4*(F186-F185)/5+F185</f>
+        <v>7.51</v>
       </c>
     </row>
   </sheetData>
@@ -76618,5 +76667,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>